<commit_message>
Driverscript changes with proceed on fail status as Critical
</commit_message>
<xml_diff>
--- a/src/main/java/com/cdp/InputFiles/CustomerPortal.xlsx
+++ b/src/main/java/com/cdp/InputFiles/CustomerPortal.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="115">
   <si>
     <t>Proceed_ON_FAIL</t>
   </si>
@@ -354,6 +354,15 @@
   </si>
   <si>
     <t>To validate save button text</t>
+  </si>
+  <si>
+    <t>CRITICAL</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Password</t>
   </si>
 </sst>
 </file>
@@ -907,7 +916,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -985,7 +994,7 @@
   <dimension ref="A1:H251"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1262,7 +1271,7 @@
         <v>55</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>65</v>
+        <v>113</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>69</v>
@@ -1310,7 +1319,7 @@
         <v>55</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>66</v>
+        <v>114</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>70</v>
@@ -1343,7 +1352,7 @@
         <v>3</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>11</v>
+        <v>112</v>
       </c>
     </row>
     <row r="16" spans="1:8">

</xml_diff>